<commit_message>
I've implemented the GUI and its different methods. Since I started with this project, I used to create a new connection whenever I want to interact with the db. It could have been a good practice or not, either way I definitely changed my way of thinking. I'm now adapting the app to fit that constraint (Only one connection throughout an execution). Till now, everything works perfectly.
</commit_message>
<xml_diff>
--- a/src/panda/host/config/sample.xlsx
+++ b/src/panda/host/config/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\IdeaProjects\Panda\pandaHost\src\panda\host\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F82419-4523-4A5F-B7C8-EDADBE0ECF54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A334B6F-6BB7-4B6B-A624-126FF4927963}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="408" windowWidth="15648" windowHeight="9732" xr2:uid="{98CA510B-6A55-49FC-B684-97295D4C1D0C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>EMAIL</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>mbappe.frank18@myiuc.com</t>
+  </si>
+  <si>
+    <t>IUC18E0036468</t>
   </si>
 </sst>
 </file>
@@ -493,15 +499,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E729E10F-064E-41DA-B2E0-BD80063233D6}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -515,117 +521,126 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{76661131-3E57-4174-A70E-2C099330F7CA}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{77F1A549-FEDE-412F-8562-4AAD85F1DB81}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{5ADAFD8D-5B8B-4617-A722-2DF9851C235A}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{9E9827DD-B5D5-4350-9305-EC5235C58E6D}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{CC995777-38CC-4420-B767-02D74180B1FA}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{67D338F8-02B5-4562-A003-1DA6C7E7D544}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{22049605-E1FB-4832-9CC6-1D4A68F550CA}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{D072E35B-6295-482E-B42E-CA01DF80824A}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{19306536-F46A-427B-B731-324DA9CC2968}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{595A4A07-8E72-4C89-8D0A-3667EFE89539}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{D23F1519-485A-4432-B8F5-310F347AE82A}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{6126FB82-1FD0-4DDC-A05E-CCF4E870920B}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{76661131-3E57-4174-A70E-2C099330F7CA}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{77F1A549-FEDE-412F-8562-4AAD85F1DB81}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{5ADAFD8D-5B8B-4617-A722-2DF9851C235A}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{9E9827DD-B5D5-4350-9305-EC5235C58E6D}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{CC995777-38CC-4420-B767-02D74180B1FA}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{67D338F8-02B5-4562-A003-1DA6C7E7D544}"/>
+    <hyperlink ref="A9" r:id="rId7" xr:uid="{22049605-E1FB-4832-9CC6-1D4A68F550CA}"/>
+    <hyperlink ref="A10" r:id="rId8" xr:uid="{D072E35B-6295-482E-B42E-CA01DF80824A}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{19306536-F46A-427B-B731-324DA9CC2968}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{595A4A07-8E72-4C89-8D0A-3667EFE89539}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{D23F1519-485A-4432-B8F5-310F347AE82A}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{6126FB82-1FD0-4DDC-A05E-CCF4E870920B}"/>
+    <hyperlink ref="A2" r:id="rId13" xr:uid="{181E9DC3-9D5E-4CB0-8AB1-069B177CA8FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>